<commit_message>
update script and add results
</commit_message>
<xml_diff>
--- a/baseline/gemini/template.xlsx
+++ b/baseline/gemini/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\0_App_Development_Folder\Playwright_Crawler_New\baseline\gemini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A719D60A-9023-40AF-864C-FE40C88B2E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D894CA1-AD89-41BC-BFF3-68808EAA11AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8192" uniqueCount="4387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8193" uniqueCount="4387">
   <si>
     <t>Date (of Dataset)</t>
   </si>
@@ -13333,13 +13333,13 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -13562,7 +13562,7 @@
   <dimension ref="A1:P1634"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -13591,7 +13591,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -13673,7 +13673,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="str">
-        <f t="shared" ref="L2:L65" si="0">IF(OR(D3="Indeterminate",F3="Indeterminate"),"Indeterminate",IF(OR(D3="Payload exceeds limit",F3="Payload exceeds limit"),"Payload exceeds limit",IF(OR(D3="Error Occurred",F3="Error Occurred"),"Error Occurred",IF(D3=F3,"Yes","No"))))</f>
+        <f t="shared" ref="L3:L65" si="0">IF(OR(D3="Indeterminate",F3="Indeterminate"),"Indeterminate",IF(OR(D3="Payload exceeds limit",F3="Payload exceeds limit"),"Payload exceeds limit",IF(OR(D3="Error Occurred",F3="Error Occurred"),"Error Occurred",IF(D3=F3,"Yes","No"))))</f>
         <v>No</v>
       </c>
     </row>
@@ -13864,10 +13864,10 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-      <c r="N10" s="16" t="s">
+      <c r="N10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O10" s="17"/>
+      <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:16" ht="12.75" customHeight="1">
       <c r="A11" s="3" t="s">
@@ -14307,10 +14307,10 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-      <c r="N24" s="16" t="s">
+      <c r="N24" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="O24" s="17"/>
+      <c r="O24" s="18"/>
     </row>
     <row r="25" spans="1:16" ht="12.75" customHeight="1">
       <c r="A25" s="3" t="s">
@@ -14450,11 +14450,11 @@
         <v>No</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="O28">
-        <f>SUM(O25:O27)</f>
-        <v>1632</v>
+        <v>4383</v>
+      </c>
+      <c r="O28" s="6">
+        <f>COUNTIF(L:L, "Error Occurred") + COUNTIF(L:L, "Payload exceeds limit")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="12.75" customHeight="1">
@@ -14482,6 +14482,13 @@
       <c r="L29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O29">
+        <f>SUM(O25:O28)</f>
+        <v>1632</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="12.75" customHeight="1">

</xml_diff>